<commit_message>
Modified Demo 3 (code, schematic, and input data)
</commit_message>
<xml_diff>
--- a/gams_demo_suite/Demo3/network_3_scematic.xlsx
+++ b/gams_demo_suite/Demo3/network_3_scematic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="108" windowWidth="10500" windowHeight="3456"/>
+    <workbookView xWindow="285" yWindow="105" windowWidth="10500" windowHeight="3450"/>
   </bookViews>
   <sheets>
     <sheet name="Schematic" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Surface reservoir</t>
   </si>
@@ -40,13 +40,19 @@
     <t>Desal plant</t>
   </si>
   <si>
-    <t>Waste water treatment plant</t>
-  </si>
-  <si>
     <t xml:space="preserve">Boundary condition </t>
   </si>
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t>WT1</t>
+  </si>
+  <si>
+    <t>Water treatment plant</t>
+  </si>
+  <si>
+    <t>Environmental flow discharge</t>
   </si>
 </sst>
 </file>
@@ -64,6 +70,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -110,13 +117,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>144780</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
@@ -158,13 +165,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
@@ -251,13 +258,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>281940</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>129540</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
@@ -296,13 +303,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>411480</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>251460</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
@@ -341,13 +348,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>441960</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>281940</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
@@ -386,13 +393,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
@@ -431,13 +438,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>556260</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -479,13 +486,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -527,13 +534,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>594360</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
@@ -575,13 +582,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>579120</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>106680</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
@@ -661,13 +668,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
@@ -709,16 +716,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>167641</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:rowOff>37148</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
+      <xdr:colOff>571501</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:rowOff>37148</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -729,8 +736,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5105400" y="396240"/>
-          <a:ext cx="1005840" cy="0"/>
+          <a:off x="4930141" y="370523"/>
+          <a:ext cx="403860" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -802,13 +809,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>441960</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
@@ -847,16 +854,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>130968</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>141923</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>171925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -867,8 +874,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="5044440" y="525780"/>
-          <a:ext cx="1287780" cy="457200"/>
+          <a:off x="5488781" y="475298"/>
+          <a:ext cx="1231582" cy="524827"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -915,8 +922,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="129540" y="605790"/>
-          <a:ext cx="396240" cy="373380"/>
+          <a:off x="129540" y="591503"/>
+          <a:ext cx="396240" cy="363855"/>
           <a:chOff x="97" y="231"/>
           <a:chExt cx="47" cy="40"/>
         </a:xfrm>
@@ -1083,13 +1090,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>594360</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
@@ -1103,8 +1110,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6389370" y="933450"/>
-          <a:ext cx="396240" cy="373380"/>
+          <a:off x="6746558" y="909638"/>
+          <a:ext cx="396240" cy="363855"/>
           <a:chOff x="97" y="231"/>
           <a:chExt cx="47" cy="40"/>
         </a:xfrm>
@@ -1271,13 +1278,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>213360</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
@@ -1319,13 +1326,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>449580</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
@@ -1370,13 +1377,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>160020</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
@@ -1390,8 +1397,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3667125" y="2045970"/>
-          <a:ext cx="207645" cy="228600"/>
+          <a:off x="4143375" y="1993583"/>
+          <a:ext cx="183833" cy="219075"/>
           <a:chOff x="27" y="294"/>
           <a:chExt cx="24" cy="24"/>
         </a:xfrm>
@@ -1457,13 +1464,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>487680</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1525,8 +1532,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="228600" y="2202180"/>
-          <a:ext cx="205740" cy="236220"/>
+          <a:off x="228600" y="2145030"/>
+          <a:ext cx="205740" cy="226695"/>
           <a:chOff x="27" y="294"/>
           <a:chExt cx="24" cy="24"/>
         </a:xfrm>
@@ -1637,14 +1644,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>61898</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>23798</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1655,8 +1662,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="236220" y="3223260"/>
-          <a:ext cx="114300" cy="129540"/>
+          <a:off x="236220" y="3895711"/>
+          <a:ext cx="114300" cy="128587"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1683,13 +1690,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>525780</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
@@ -1731,28 +1738,71 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="Line 48"/>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Oval 49"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4221480" y="3589020"/>
+          <a:ext cx="144780" cy="160020"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Line 50"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="4998720" y="1333500"/>
-          <a:ext cx="106680" cy="129540"/>
+          <a:off x="4290060" y="3764280"/>
+          <a:ext cx="7620" cy="739140"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1780,70 +1830,27 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Oval 49"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4221480" y="3589020"/>
-          <a:ext cx="144780" cy="160020"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="Line 50"/>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Line 51"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="4290060" y="3764280"/>
-          <a:ext cx="7620" cy="739140"/>
+          <a:off x="3383280" y="2781300"/>
+          <a:ext cx="807720" cy="327660"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1870,62 +1877,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="Line 51"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="1">
-          <a:off x="3383280" y="2781300"/>
-          <a:ext cx="807720" cy="327660"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:noFill/>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>138589</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>589121</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1938,8 +1897,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6134100" y="243840"/>
-          <a:ext cx="472440" cy="259080"/>
+          <a:off x="6091714" y="242888"/>
+          <a:ext cx="450532" cy="257175"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1961,13 +1920,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>205740</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
@@ -1981,8 +1940,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2276475" y="3535680"/>
-          <a:ext cx="405765" cy="381000"/>
+          <a:off x="2800350" y="3440430"/>
+          <a:ext cx="381953" cy="371475"/>
           <a:chOff x="97" y="231"/>
           <a:chExt cx="47" cy="40"/>
         </a:xfrm>
@@ -2149,13 +2108,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>160020</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>441960</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
@@ -2197,13 +2156,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>201930</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>120015</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>544830</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>20955</xdr:rowOff>
@@ -2248,13 +2207,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>510540</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
@@ -2296,13 +2255,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>556260</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>411480</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
@@ -2339,16 +2298,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
+      <xdr:colOff>107157</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>121919</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2359,8 +2318,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="4434840" y="2651760"/>
-          <a:ext cx="1638300" cy="152400"/>
+          <a:off x="4281489" y="2762249"/>
+          <a:ext cx="588168" cy="26670"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2387,13 +2346,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>312420</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>487680</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
@@ -2477,13 +2436,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>106680</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
@@ -2525,13 +2484,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>449580</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
@@ -2576,155 +2535,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="69" name="Line 68"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="1">
-          <a:off x="3116580" y="2918460"/>
-          <a:ext cx="106680" cy="129540"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:noFill/>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="70" name="Line 69"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="1">
-          <a:off x="5699760" y="2811780"/>
-          <a:ext cx="632460" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:noFill/>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="71" name="AutoShape 70"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5494020" y="3017520"/>
-          <a:ext cx="175260" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="octagon">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 29287"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>59530</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
@@ -2737,8 +2555,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="4396740" y="3185160"/>
-          <a:ext cx="1120140" cy="434340"/>
+          <a:off x="4838699" y="2809875"/>
+          <a:ext cx="1769269" cy="789623"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2768,28 +2586,217 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="73" name="Line 72"/>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="74" name="AutoShape 73"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2926080" y="4030980"/>
+          <a:ext cx="464820" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="75" name="Line 74"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
-        <a:xfrm flipV="1">
-          <a:off x="5661660" y="2773680"/>
-          <a:ext cx="541020" cy="251460"/>
+        <a:xfrm flipH="1">
+          <a:off x="3398520" y="3749040"/>
+          <a:ext cx="815340" cy="312420"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:noFill/>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="76" name="Line 75"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeShapeType="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3383280" y="4229100"/>
+          <a:ext cx="845820" cy="365760"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:noFill/>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="Line 76"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeShapeType="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2682240" y="3726180"/>
+          <a:ext cx="243840" cy="320040"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:noFill/>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>192405</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>135255</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>150495</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="78" name="Line 77"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeShapeType="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2668905" y="3907155"/>
+          <a:ext cx="274320" cy="358140"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2819,33 +2826,31 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="74" name="AutoShape 73"/>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="79" name="Oval 78"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2926080" y="4030980"/>
-          <a:ext cx="464820" cy="236220"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 16667"/>
-          </a:avLst>
+          <a:off x="4229100" y="4518660"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
@@ -2864,347 +2869,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="75" name="Line 74"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="1">
-          <a:off x="3398520" y="3749040"/>
-          <a:ext cx="815340" cy="312420"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:noFill/>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="76" name="Line 75"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3383280" y="4229100"/>
-          <a:ext cx="845820" cy="365760"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:noFill/>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="77" name="Line 76"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="2682240" y="3726180"/>
-          <a:ext cx="243840" cy="320040"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:noFill/>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>192405</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>135255</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>150495</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="78" name="Line 77"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2668905" y="3907155"/>
-          <a:ext cx="274320" cy="358140"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-        <a:extLst/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="79" name="Oval 78"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4229100" y="4518660"/>
-          <a:ext cx="152400" cy="152400"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="80" name="Line 79"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="1">
-          <a:off x="6690360" y="777240"/>
-          <a:ext cx="121920" cy="137160"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:noFill/>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="81" name="Line 80"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="1">
-          <a:off x="2362200" y="3322320"/>
-          <a:ext cx="106680" cy="129540"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:noFill/>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>521970</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>264795</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>93504</xdr:rowOff>
@@ -3260,13 +2931,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>405765</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>133588</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>142948</xdr:rowOff>
@@ -3322,14 +2993,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>520065</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>472441</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>93345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>247888</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200264</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
@@ -3342,8 +3013,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4840605" y="1602105"/>
-          <a:ext cx="345043" cy="196215"/>
+          <a:off x="4639629" y="1593533"/>
+          <a:ext cx="323135" cy="195262"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3384,13 +3055,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>443865</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>93345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>169545</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>104927</xdr:rowOff>
@@ -3446,13 +3117,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>236220</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>577172</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -3508,14 +3179,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>171447</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>379095</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>521967</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>131674</xdr:rowOff>
     </xdr:to>
@@ -3528,8 +3199,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6200775" y="262890"/>
-          <a:ext cx="350520" cy="204064"/>
+          <a:off x="6124572" y="261938"/>
+          <a:ext cx="350520" cy="203111"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3570,13 +3241,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>605790</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>340954</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>93574</xdr:rowOff>
@@ -3632,13 +3303,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>483870</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>93345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>226695</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>104927</xdr:rowOff>
@@ -3694,13 +3365,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>434340</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>169504</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -3756,13 +3427,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>510540</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>236220</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -3818,75 +3489,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>520065</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>407754</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="92" name="Text Box 91"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5457825" y="3232785"/>
-          <a:ext cx="504909" cy="196215"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF">
-            <a:alpha val="0"/>
-          </a:srgbClr>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="0" anchor="t" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l" rtl="1">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>WWTP1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>142948</xdr:rowOff>
@@ -3942,13 +3551,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>405765</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -4004,13 +3613,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>131674</xdr:rowOff>
@@ -4066,13 +3675,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>274254</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -4128,13 +3737,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>131445</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>131445</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>407670</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>143027</xdr:rowOff>
@@ -4190,28 +3799,28 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="98" name="Line 98"/>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>103332</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>103332</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="100" name="Line 100"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="1">
-          <a:off x="4366260" y="4396740"/>
-          <a:ext cx="121920" cy="129540"/>
+        <a:xfrm>
+          <a:off x="144780" y="4270520"/>
+          <a:ext cx="297180" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4238,73 +3847,28 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>584561</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="99" name="AutoShape 99"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="213360" y="2849880"/>
-          <a:ext cx="175260" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="octagon">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 29287"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="100" name="Line 100"/>
+      <xdr:rowOff>71845</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>402770</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="101" name="Line 46"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="144780" y="3611880"/>
-          <a:ext cx="297180" cy="0"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7409904" y="3010988"/>
+          <a:ext cx="438695" cy="265612"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4331,28 +3895,81 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>559594</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>83342</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>154782</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Regular Pentagon 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5322094" y="250030"/>
+          <a:ext cx="345281" cy="238127"/>
+        </a:xfrm>
+        <a:prstGeom prst="pentagon">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="3175"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>320028</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>34770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>584561</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>71845</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>402770</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>10886</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="101" name="Line 46"/>
+      <xdr:colOff>128576</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>34770</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="102" name="Line 14"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="7409904" y="3010988"/>
-          <a:ext cx="438695" cy="265612"/>
+        <a:xfrm>
+          <a:off x="5677841" y="368145"/>
+          <a:ext cx="403860" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4374,6 +3991,439 @@
           </a:ext>
         </a:extLst>
       </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>450056</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>33338</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="103" name="Regular Pentagon 102"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4867275" y="2628899"/>
+          <a:ext cx="345281" cy="238127"/>
+        </a:xfrm>
+        <a:prstGeom prst="pentagon">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="3175"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>445295</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>583406</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>48099</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="104" name="Line 63"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeShapeType="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipV="1">
+          <a:off x="5207795" y="2690812"/>
+          <a:ext cx="733424" cy="24287"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:noFill/>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>511969</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>130971</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="TextBox 20"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4762500" y="2881314"/>
+          <a:ext cx="511969" cy="250032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>WT2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>107157</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>452438</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47627</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="110" name="Regular Pentagon 109"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="107157" y="3143250"/>
+          <a:ext cx="345281" cy="238127"/>
+        </a:xfrm>
+        <a:prstGeom prst="pentagon">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="3175"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>440534</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95258</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>130971</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47633</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Diamond 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4012409" y="4929196"/>
+          <a:ext cx="285750" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="3175"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>589121</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>7</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>589121</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="111" name="Line 10"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeShapeType="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="1">
+          <a:off x="4160996" y="4667257"/>
+          <a:ext cx="0" cy="273837"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:noFill/>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>166684</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142871</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>11905</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="112" name="Text Box 95"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4333872" y="4976809"/>
+          <a:ext cx="476254" cy="202409"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:alpha val="0"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="1">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>EndPt</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>154778</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>154782</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>440528</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>107157</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="113" name="Diamond 112"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="154778" y="3488532"/>
+          <a:ext cx="285750" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="3175"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -4667,93 +4717,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R22"/>
+  <dimension ref="B2:S24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="O3" s="2"/>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="P4" s="2"/>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="K4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="P6" s="2"/>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="P7" s="2"/>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="P9" s="2"/>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="P11" s="2"/>
-      <c r="R11" s="1" t="s">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q11" s="2"/>
+      <c r="S11" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="P13" s="2"/>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>